<commit_message>
fix stack overvlow issue
</commit_message>
<xml_diff>
--- a/src/resources/excelSource/Ho-ho-ho.xlsx
+++ b/src/resources/excelSource/Ho-ho-ho.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmosin\OneDrive - ENDAVA\Desktop\GIT\SecretSanta\src\resources\excelSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://endava-my.sharepoint.com/personal/gheorghii_mosin_endava_com/Documents/Desktop/SecretSanta/src/resources/excelSource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB727009-5F4C-400D-8244-6AA4340C3397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{BB727009-5F4C-400D-8244-6AA4340C3397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610BD99E-9AC0-40BE-8623-B399532FDD9D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -70,6 +81,114 @@
   </si>
   <si>
     <t>John Johns</t>
+  </si>
+  <si>
+    <t>Bob.Ross@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Johny,Silverhand@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Bob Ross</t>
+  </si>
+  <si>
+    <t>Johny Silverhand</t>
+  </si>
+  <si>
+    <t>Alistor.Radiodemon@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Alistor Radiodemon</t>
+  </si>
+  <si>
+    <t>Victor.Vector@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Victor Vector</t>
+  </si>
+  <si>
+    <t>Judi.Alvarez@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Eveline.Parker@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Dexter.Deshawn@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Johny.Welles@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Lizzy.Wizzy@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Regina.Johns@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Wakako.Asada@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Yorinobu.Arasaka@PotatoFest.com</t>
+  </si>
+  <si>
+    <t>Judi Alvarez</t>
+  </si>
+  <si>
+    <t>Eveline Parker</t>
+  </si>
+  <si>
+    <t>Dexter Deshawn</t>
+  </si>
+  <si>
+    <t>Johny Welles</t>
+  </si>
+  <si>
+    <t>Lizzy Wizzy</t>
+  </si>
+  <si>
+    <t>Regina Johns</t>
+  </si>
+  <si>
+    <t>Wakako Asada</t>
+  </si>
+  <si>
+    <t>Yorinobu Arasaka</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>Chaos</t>
+  </si>
+  <si>
+    <t>Orthans</t>
+  </si>
+  <si>
+    <t>Boxing</t>
+  </si>
+  <si>
+    <t>BDs</t>
+  </si>
+  <si>
+    <t>Smokes</t>
+  </si>
+  <si>
+    <t>Peace and Quite</t>
+  </si>
+  <si>
+    <t>Misty ;)</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Traditional Jappanese tea</t>
+  </si>
+  <si>
+    <t>Engrams</t>
   </si>
 </sst>
 </file>
@@ -120,14 +239,14 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -139,6 +258,40 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
@@ -163,16 +316,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0">
-  <autoFilter ref="A1:G4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G17" totalsRowCount="1">
+  <autoFilter ref="A1:G16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completion time" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="0" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Do you want to be someone's Secret Santa?" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="These are a few of my favorite things:" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completion time" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Do you want to be someone's Secret Santa?" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="These are a few of my favorite things:" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -475,38 +628,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="64" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -520,16 +675,16 @@
       <c r="C2" s="1">
         <v>44896.504675925898</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -543,16 +698,16 @@
       <c r="C3" s="1">
         <v>44896.505127314798</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -566,29 +721,333 @@
       <c r="C4" s="1">
         <v>44896.505902777797</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>A4+1</f>
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44897.504201388889</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A5+1</f>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44898.504201388889</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ref="A7:A16" si="0">A6+1</f>
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44899.504201388889</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44900.504201388889</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44901.504201388889</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44902.504201388889</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44903.504201388889</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44904.504201388889</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44905.504201388889</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44906.504201388889</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44907.504201388889</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44908.504201388889</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44896.505902777797</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{B5413053-68A7-4FB1-A376-60FB165CDA4C}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{8E8E1A14-0BE2-445C-A728-303F9485828C}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{2E8AA15D-B3A9-4D88-81E4-EF2A31F5B20B}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{73559839-3D05-4F89-9326-B99B428D2E89}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{CB74D204-6AE1-4844-99AE-2A6BA5DF40E9}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{453CF3EE-CE37-4824-A1E7-67D16CB5B66B}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{9DCEADC3-8CE3-48BA-B503-69EAAFAF7BD0}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{F4539DB6-7E82-491F-9F0A-051D6B982460}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{8DC8B2E5-F812-4F39-9E77-B944C14FA34B}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{33806590-7B64-48CA-9482-E209A190636C}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{3F9CA097-12C0-4324-B13D-642D8A15BF20}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{92419039-6E1D-45C7-AA6A-95C3BC65E4CB}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{1D7F578A-FD39-4C98-9E57-B9A0C9C3B0DB}"/>
+    <hyperlink ref="D16" r:id="rId14" xr:uid="{94A1D48B-5182-463D-B1AE-BA6B7A888590}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>